<commit_message>
Update and add encoder, decode for mqtt message.
</commit_message>
<xml_diff>
--- a/99_Reference/Accton/Command Definition.xlsx
+++ b/99_Reference/Accton/Command Definition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen.Chen\source\repos\0925_Smart Chamber\99_Reference\Accton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\0926_MQTT Study\99_Reference\Accton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E37E4C-CD9E-4CE9-8059-48FC1D0B6DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD7EB31-B4CD-4282-84E8-5733564AEB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15935" xr2:uid="{3519653B-91D5-4E24-9457-54DBB83227BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3519653B-91D5-4E24-9457-54DBB83227BD}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>[Topic Name] Detail - CMD#</t>
   </si>
@@ -63,43 +63,272 @@
   </si>
   <si>
     <t>CMD#</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Get Test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SET_RACK_STATUS</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MQTT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Online Request</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Register MQTT Topic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for Communication</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Publish </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Current Station Status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Maintain, Open, Close</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Query the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DUT Test Result</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: DUT, FAIL</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Send </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Power-On Command to Fixture</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ack the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DUT Feed-In</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Abnormal Handling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Force DUT Out</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Send </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WILL Message</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="22"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="32"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,25 +360,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -181,9 +426,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>590516</xdr:colOff>
+      <xdr:colOff>580991</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>388189</xdr:rowOff>
+      <xdr:rowOff>397714</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -536,279 +781,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27E4CAF-2490-4282-ADDC-846A58C57E5E}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="28.55" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="9" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="11" max="12" width="21.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="7.625" customWidth="1"/>
+    <col min="10" max="10" width="10.375" style="4" customWidth="1"/>
+    <col min="11" max="12" width="21.25" style="3" customWidth="1"/>
     <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="8.875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="17.375" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="47.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J2" s="3">
+    <row r="2" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="5">
         <v>0</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="K2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="N2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J3" s="3">
+      <c r="P2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="5">
         <v>0</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="K3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J4" s="3">
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="5">
         <v>1</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J5" s="3">
+      <c r="K4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5" s="5">
         <v>1</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J6" s="3">
+      <c r="K5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="5">
         <v>3</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J7" s="3">
+      <c r="K6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="5">
         <v>3</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J8" s="3">
+      <c r="K7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="5">
         <v>6</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J9" s="3">
+      <c r="K8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="5">
         <v>6</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J10" s="3">
+      <c r="K9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="5">
         <v>6</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J11" s="3">
+      <c r="K10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="5">
         <v>9</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J12" s="3">
+      <c r="K11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="5">
         <v>9</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J13" s="3">
+      <c r="K12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="5">
         <v>23</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J14" s="3">
+      <c r="K13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="5">
         <v>23</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J15" s="3">
+      <c r="K14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="5">
         <v>24</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J16" s="3">
+      <c r="K15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="5">
         <v>24</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J17" s="3">
+      <c r="K16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="5">
         <v>25</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J18" s="3">
+      <c r="K17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="5">
         <v>25</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="J19" s="3">
+      <c r="K18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="5">
         <v>65535</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="21" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="22" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="23" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="24" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="25" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="26" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="27" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="28" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="29" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="30" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="31" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="32" spans="10:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="33" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="34" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="35" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="36" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5"/>
+      <c r="K19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="26" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="29" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="30" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="32" spans="10:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="33" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="34" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="K2:L19">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"AGT"</formula>

</xml_diff>